<commit_message>
Initial commit for Heroku deployment
</commit_message>
<xml_diff>
--- a/uploads/summary_report_with_graphs.xlsx
+++ b/uploads/summary_report_with_graphs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Month</t>
   </si>
@@ -25,7 +25,40 @@
     <t>Credit</t>
   </si>
   <si>
-    <t>2025-10</t>
+    <t>2024-10</t>
+  </si>
+  <si>
+    <t>2024-11</t>
+  </si>
+  <si>
+    <t>2024-12</t>
+  </si>
+  <si>
+    <t>2025-01</t>
+  </si>
+  <si>
+    <t>2025-02</t>
+  </si>
+  <si>
+    <t>2025-03</t>
+  </si>
+  <si>
+    <t>2025-04</t>
+  </si>
+  <si>
+    <t>2025-05</t>
+  </si>
+  <si>
+    <t>2025-06</t>
+  </si>
+  <si>
+    <t>2025-07</t>
+  </si>
+  <si>
+    <t>2025-08</t>
+  </si>
+  <si>
+    <t>2025-09</t>
   </si>
 </sst>
 </file>
@@ -104,13 +137,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>362719</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -128,7 +161,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="571500"/>
+          <a:off x="0" y="2667000"/>
           <a:ext cx="3410719" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -142,18 +175,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>25913</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>362719</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="monthly_summary.png"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="debit_credit_pie.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -166,8 +199,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="5334000"/>
-          <a:ext cx="4521717" cy="2692913"/>
+          <a:off x="0" y="8382000"/>
+          <a:ext cx="3410719" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -180,18 +213,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>259089</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>25913</xdr:rowOff>
+      <xdr:colOff>254517</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="cumulative_balance.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="income_expense_trend.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -204,121 +237,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="10096500"/>
-          <a:ext cx="4526289" cy="2692913"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>277377</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>178315</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="top_10_spending.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="14859000"/>
-          <a:ext cx="4544577" cy="3607315"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>568459</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>166122</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="debit_credit_pie.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="20574000"/>
-          <a:ext cx="3616459" cy="3214122"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>30485</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="day_of_week_spending.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="26289000"/>
+          <a:off x="0" y="14097000"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -332,18 +251,132 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>163</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="income_expense_trend.png"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="day_of_week_spending.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="18859500"/>
+          <a:ext cx="4521717" cy="2697485"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254517</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>30485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="monthly_summary.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="23622000"/>
+          <a:ext cx="4521717" cy="2697485"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254517</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>30485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="cumulative_balance.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28384500"/>
+          <a:ext cx="4521717" cy="2697485"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>286521</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>178315</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="top_10_spending.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -356,8 +389,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="31051500"/>
-          <a:ext cx="4521717" cy="2697485"/>
+          <a:off x="0" y="33147000"/>
+          <a:ext cx="4553721" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -654,7 +687,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -676,10 +709,131 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>863.54</v>
+        <v>4027</v>
       </c>
       <c r="C2">
-        <v>22</v>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>10680</v>
+      </c>
+      <c r="C3">
+        <v>5612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>13780.71</v>
+      </c>
+      <c r="C4">
+        <v>9106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>8565.16</v>
+      </c>
+      <c r="C5">
+        <v>18470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>5289.09</v>
+      </c>
+      <c r="C6">
+        <v>11777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>9220.440000000001</v>
+      </c>
+      <c r="C7">
+        <v>5948</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>7251.12</v>
+      </c>
+      <c r="C8">
+        <v>16442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>11937.29</v>
+      </c>
+      <c r="C9">
+        <v>11183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>9805.360000000001</v>
+      </c>
+      <c r="C10">
+        <v>11057</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>99163.04000000001</v>
+      </c>
+      <c r="C11">
+        <v>100539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>9943.039999999999</v>
+      </c>
+      <c r="C12">
+        <v>9210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>11499.36</v>
+      </c>
+      <c r="C13">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new features and update design
</commit_message>
<xml_diff>
--- a/uploads/summary_report_with_graphs.xlsx
+++ b/uploads/summary_report_with_graphs.xlsx
@@ -137,13 +137,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>362719</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -161,7 +161,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2667000"/>
+          <a:off x="0" y="3048000"/>
           <a:ext cx="3410719" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -173,15 +173,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>362719</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -199,7 +199,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="8382000"/>
+          <a:off x="6096000" y="3048000"/>
           <a:ext cx="3410719" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -213,13 +213,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -237,7 +237,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="14097000"/>
+          <a:off x="0" y="9144000"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -249,15 +249,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -275,7 +275,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="18859500"/>
+          <a:off x="6096000" y="9144000"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -289,13 +289,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -313,7 +313,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="23622000"/>
+          <a:off x="0" y="14287500"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -325,15 +325,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>149</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>163</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -351,7 +351,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="28384500"/>
+          <a:off x="6096000" y="14287500"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -365,13 +365,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>286521</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -389,7 +389,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="33147000"/>
+          <a:off x="0" y="19431000"/>
           <a:ext cx="4553721" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>

<commit_message>
Initial commit of Flask statement analyzer
</commit_message>
<xml_diff>
--- a/uploads/summary_report_with_graphs.xlsx
+++ b/uploads/summary_report_with_graphs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Month</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>2025-09</t>
+  </si>
+  <si>
+    <t>2025-10</t>
   </si>
 </sst>
 </file>
@@ -137,13 +140,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>362719</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>237752</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -161,8 +164,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3048000"/>
-          <a:ext cx="3410719" cy="3607315"/>
+          <a:off x="0" y="3238500"/>
+          <a:ext cx="3895352" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -175,14 +178,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>362719</xdr:colOff>
+      <xdr:colOff>522739</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>178315</xdr:rowOff>
+      <xdr:rowOff>172219</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -199,8 +202,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="3048000"/>
-          <a:ext cx="3410719" cy="3607315"/>
+          <a:off x="6096000" y="3238500"/>
+          <a:ext cx="3570739" cy="3410719"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -213,13 +216,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -237,7 +240,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="9144000"/>
+          <a:off x="0" y="9334500"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -251,13 +254,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -275,7 +278,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="9144000"/>
+          <a:off x="6096000" y="9334500"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -289,13 +292,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:colOff>245373</xdr:colOff>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -313,8 +316,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="14287500"/>
-          <a:ext cx="4521717" cy="2697485"/>
+          <a:off x="0" y="14478000"/>
+          <a:ext cx="4512573" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -327,13 +330,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:colOff>245373</xdr:colOff>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -351,8 +354,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="14287500"/>
-          <a:ext cx="4521717" cy="2697485"/>
+          <a:off x="6096000" y="14478000"/>
+          <a:ext cx="4512573" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -365,13 +368,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>286521</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -389,7 +392,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19431000"/>
+          <a:off x="0" y="19621500"/>
           <a:ext cx="4553721" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -687,7 +690,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -709,10 +712,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4027</v>
+        <v>9309</v>
       </c>
       <c r="C2">
-        <v>330</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -720,10 +723,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>10680</v>
+        <v>61830.84</v>
       </c>
       <c r="C3">
-        <v>5612</v>
+        <v>1278.18</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -731,10 +734,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>13780.71</v>
+        <v>39726.59</v>
       </c>
       <c r="C4">
-        <v>9106</v>
+        <v>7110</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -742,10 +745,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>8565.16</v>
+        <v>86781.59</v>
       </c>
       <c r="C5">
-        <v>18470</v>
+        <v>18200</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -753,10 +756,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>5289.09</v>
+        <v>176843.95</v>
       </c>
       <c r="C6">
-        <v>11777</v>
+        <v>35528</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -764,10 +767,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>9220.440000000001</v>
+        <v>24830</v>
       </c>
       <c r="C7">
-        <v>5948</v>
+        <v>6549.99</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -775,10 +778,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>7251.12</v>
+        <v>30579.5</v>
       </c>
       <c r="C8">
-        <v>16442</v>
+        <v>7194.5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -786,10 +789,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>11937.29</v>
+        <v>31874</v>
       </c>
       <c r="C9">
-        <v>11183</v>
+        <v>6669</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -797,10 +800,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>9805.360000000001</v>
+        <v>91630</v>
       </c>
       <c r="C10">
-        <v>11057</v>
+        <v>19965.31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -808,10 +811,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>99163.04000000001</v>
+        <v>201555.02</v>
       </c>
       <c r="C11">
-        <v>100539</v>
+        <v>7265.53</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -819,10 +822,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>9943.039999999999</v>
+        <v>24919</v>
       </c>
       <c r="C12">
-        <v>9210</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -830,10 +833,21 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>11499.36</v>
+        <v>3299</v>
       </c>
       <c r="C13">
-        <v>430</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>19477</v>
+      </c>
+      <c r="C14">
+        <v>7378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Google AdSense code to index.html for monetization setup
</commit_message>
<xml_diff>
--- a/uploads/summary_report_with_graphs.xlsx
+++ b/uploads/summary_report_with_graphs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Month</t>
   </si>
@@ -23,42 +23,6 @@
   </si>
   <si>
     <t>Credit</t>
-  </si>
-  <si>
-    <t>2024-10</t>
-  </si>
-  <si>
-    <t>2024-11</t>
-  </si>
-  <si>
-    <t>2024-12</t>
-  </si>
-  <si>
-    <t>2025-01</t>
-  </si>
-  <si>
-    <t>2025-02</t>
-  </si>
-  <si>
-    <t>2025-03</t>
-  </si>
-  <si>
-    <t>2025-04</t>
-  </si>
-  <si>
-    <t>2025-05</t>
-  </si>
-  <si>
-    <t>2025-06</t>
-  </si>
-  <si>
-    <t>2025-07</t>
-  </si>
-  <si>
-    <t>2025-08</t>
-  </si>
-  <si>
-    <t>2025-09</t>
   </si>
   <si>
     <t>2025-10</t>
@@ -140,13 +104,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>237752</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>362719</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -164,8 +128,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3238500"/>
-          <a:ext cx="3895352" cy="3607315"/>
+          <a:off x="0" y="952500"/>
+          <a:ext cx="3410719" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -178,14 +142,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>522739</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>172219</xdr:rowOff>
+      <xdr:colOff>568459</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>156978</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -202,8 +166,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="3238500"/>
-          <a:ext cx="3570739" cy="3410719"/>
+          <a:off x="6096000" y="952500"/>
+          <a:ext cx="3616459" cy="3204978"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -216,13 +180,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -240,7 +204,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="9334500"/>
+          <a:off x="0" y="7048500"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -254,13 +218,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>254517</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -278,7 +242,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="9334500"/>
+          <a:off x="6096000" y="7048500"/>
           <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -292,14 +256,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>245373</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>30485</xdr:rowOff>
+      <xdr:colOff>254517</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>25913</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -316,8 +280,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="14478000"/>
-          <a:ext cx="4512573" cy="2697485"/>
+          <a:off x="0" y="12192000"/>
+          <a:ext cx="4521717" cy="2692913"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -330,13 +294,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>245373</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:colOff>254517</xdr:colOff>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>30485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -354,8 +318,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="14478000"/>
-          <a:ext cx="4512573" cy="2697485"/>
+          <a:off x="6096000" y="12192000"/>
+          <a:ext cx="4521717" cy="2697485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -368,13 +332,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>286521</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:colOff>268233</xdr:colOff>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>178315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -392,8 +356,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19621500"/>
-          <a:ext cx="4553721" cy="3607315"/>
+          <a:off x="0" y="17335500"/>
+          <a:ext cx="4535433" cy="3607315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -690,7 +654,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -712,142 +676,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>9309</v>
+        <v>5104.64</v>
       </c>
       <c r="C2">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>61830.84</v>
-      </c>
-      <c r="C3">
-        <v>1278.18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>39726.59</v>
-      </c>
-      <c r="C4">
-        <v>7110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>86781.59</v>
-      </c>
-      <c r="C5">
-        <v>18200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>176843.95</v>
-      </c>
-      <c r="C6">
-        <v>35528</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>24830</v>
-      </c>
-      <c r="C7">
-        <v>6549.99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>30579.5</v>
-      </c>
-      <c r="C8">
-        <v>7194.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>31874</v>
-      </c>
-      <c r="C9">
-        <v>6669</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>91630</v>
-      </c>
-      <c r="C10">
-        <v>19965.31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>201555.02</v>
-      </c>
-      <c r="C11">
-        <v>7265.53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>24919</v>
-      </c>
-      <c r="C12">
-        <v>3432</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>3299</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>19477</v>
-      </c>
-      <c r="C14">
-        <v>7378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>